<commit_message>
fixed all values confusion
</commit_message>
<xml_diff>
--- a/th_UNet rewrites/savedstatistics/30epoch30firstImglr1e-3AdamCrossentr.xlsx
+++ b/th_UNet rewrites/savedstatistics/30epoch30firstImglr1e-3AdamCrossentr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophanemayaud/Dev/EPFL MA1/Machine Learning/cs-433-project-2-ml_fools/th_UNet rewrites/savedstatistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophanemayaud/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1367B54F-53B0-D741-8247-67B9796642F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2814E1C0-0AC0-914A-9AD7-E66EF20A2DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11960" yWindow="5900" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="6200" yWindow="1700" windowWidth="22220" windowHeight="15740"/>
   </bookViews>
   <sheets>
     <sheet name="30epoch30firstImglr1e-3AdamCros" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <t>TP</t>
   </si>
   <si>
-    <t>FN</t>
+    <t>TN</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:C198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C198"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>